<commit_message>
Admin Local interface changes
</commit_message>
<xml_diff>
--- a/DB_Structure.xlsx
+++ b/DB_Structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MscIT_SR\sem-projects\Sem8\Synopsis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kunal\Project\The_Landmark_Tour\tlt_1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F881B83C-9B48-4C61-9011-CD4FFC0629A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF6D6BA-F5DC-482C-86E2-06244A47B7A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="91">
   <si>
     <t>Places</t>
   </si>
@@ -286,13 +286,25 @@
   </si>
   <si>
     <t>payment_method_ID(FK)</t>
+  </si>
+  <si>
+    <t>payment_Id (FK)</t>
+  </si>
+  <si>
+    <t>userId (FK)</t>
+  </si>
+  <si>
+    <t>payment_ID(FK)</t>
+  </si>
+  <si>
+    <t>AppointmentMaster</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -327,6 +339,21 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -405,7 +432,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
@@ -418,6 +445,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in 20% - Accent1" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
@@ -804,39 +842,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="114" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="27.42578125" customWidth="1"/>
-    <col min="11" max="11" width="31.5703125" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27.44140625" customWidth="1"/>
+    <col min="11" max="11" width="31.5546875" customWidth="1"/>
+    <col min="12" max="12" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="2:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="C3" s="6"/>
+      <c r="E3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="H3" s="3" t="s">
+      <c r="F3" s="6"/>
+      <c r="H3" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="K3" s="3" t="s">
+      <c r="I3" s="6"/>
+      <c r="K3" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="3"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L3" s="6"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -862,7 +900,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
@@ -888,7 +926,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
@@ -910,19 +948,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="2:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
@@ -935,8 +973,12 @@
       <c r="F8" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="2:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
@@ -949,16 +991,18 @@
       <c r="F9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" s="3"/>
-      <c r="K9" s="4" t="s">
+      <c r="H9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="L9" s="5"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L9" s="8"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
@@ -972,7 +1016,7 @@
         <v>3</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>3</v>
@@ -984,7 +1028,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
@@ -992,7 +1036,7 @@
         <v>3</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>3</v>
@@ -1004,19 +1048,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="K12" s="2" t="s">
         <v>74</v>
       </c>
@@ -1024,17 +1062,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="5"/>
+      <c r="F13" s="8"/>
+      <c r="H13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="5"/>
       <c r="K13" s="2" t="s">
         <v>75</v>
       </c>
@@ -1042,17 +1084,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E14" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H14" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I14" s="5"/>
+      <c r="H14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="K14" s="2" t="s">
         <v>76</v>
       </c>
@@ -1060,7 +1104,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E15" s="2" t="s">
         <v>39</v>
       </c>
@@ -1068,10 +1112,10 @@
         <v>3</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>77</v>
@@ -1080,11 +1124,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
+    <row r="16" spans="2:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="6"/>
       <c r="E16" s="2" t="s">
         <v>5</v>
       </c>
@@ -1092,7 +1136,7 @@
         <v>3</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>12</v>
@@ -1104,7 +1148,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1118,10 +1162,10 @@
         <v>30</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>86</v>
@@ -1130,7 +1174,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1144,13 +1188,13 @@
         <v>3</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>25</v>
       </c>
@@ -1164,13 +1208,13 @@
         <v>3</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>26</v>
       </c>
@@ -1183,36 +1227,42 @@
       <c r="F20" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
+      <c r="H20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B21" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>83</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="5"/>
-      <c r="H22" s="4" t="s">
+      <c r="F22" s="8"/>
+      <c r="H22" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I22" s="5"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
+      <c r="I22" s="8"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B23" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E23" s="2" t="s">
@@ -1228,11 +1278,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B24" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E24" s="2" t="s">
@@ -1248,7 +1298,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
         <v>82</v>
       </c>
@@ -1262,7 +1312,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
         <v>79</v>
       </c>
@@ -1276,17 +1326,17 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B27" s="2" t="s">
+    <row r="27" spans="2:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B27" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F27" s="3"/>
+      <c r="F27" s="6"/>
       <c r="H27" s="2" t="s">
         <v>64</v>
       </c>
@@ -1294,11 +1344,11 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B28" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E28" s="2" t="s">
@@ -1308,9 +1358,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>3</v>
@@ -1321,12 +1371,12 @@
       <c r="F29" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="H29" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="I29" s="5"/>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I29" s="8"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H30" s="2" t="s">
         <v>55</v>
       </c>
@@ -1334,11 +1384,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E31" s="3" t="s">
+    <row r="31" spans="2:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="E31" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F31" s="3"/>
+      <c r="F31" s="6"/>
       <c r="H31" s="2" t="s">
         <v>84</v>
       </c>
@@ -1346,11 +1396,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B32" s="4" t="s">
+    <row r="32" spans="2:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B32" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="5"/>
+      <c r="C32" s="8"/>
       <c r="E32" s="2" t="s">
         <v>34</v>
       </c>
@@ -1364,7 +1414,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
         <v>10</v>
       </c>
@@ -1378,7 +1428,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
         <v>5</v>
       </c>
@@ -1392,31 +1442,47 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E35" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H35" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="I35" s="8"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E36" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B37" s="4" t="s">
+      <c r="H36" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B37" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="5"/>
+      <c r="C37" s="8"/>
       <c r="E37"/>
       <c r="F37"/>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B38" s="2" t="s">
         <v>52</v>
       </c>
@@ -1425,8 +1491,14 @@
       </c>
       <c r="E38"/>
       <c r="F38"/>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H38" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B39" s="2" t="s">
         <v>5</v>
       </c>
@@ -1435,21 +1507,35 @@
       </c>
       <c r="E39"/>
       <c r="F39"/>
-    </row>
-    <row r="40" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="H39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E40"/>
       <c r="F40"/>
-    </row>
-    <row r="41" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="H40" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E41"/>
       <c r="F41"/>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E42"/>
       <c r="F42"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="16">
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="H35:I35"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="K9:L9"/>
     <mergeCell ref="B37:C37"/>
@@ -1457,16 +1543,13 @@
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E22:F22"/>
-    <mergeCell ref="H14:I14"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="H29:I29"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H9:I9"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="B16:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Explore place and other entity addition
</commit_message>
<xml_diff>
--- a/DB_Structure.xlsx
+++ b/DB_Structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MscIT_SR\sem-projects\Sem8\Sprint1\TheLandmarkTour\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AD2FF9-CAEB-42B7-863B-E5526842314C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7381143-8314-495C-842B-8987EFB21E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="90">
   <si>
     <t>Places</t>
   </si>
@@ -72,21 +72,9 @@
     <t>CategoryID(FK)</t>
   </si>
   <si>
-    <t>Bus stop</t>
-  </si>
-  <si>
     <t>CityID(FK)</t>
   </si>
   <si>
-    <t>StopId (PK)</t>
-  </si>
-  <si>
-    <t>StopName</t>
-  </si>
-  <si>
-    <t>BusNumber(FK)</t>
-  </si>
-  <si>
     <t>GuideID(PK)</t>
   </si>
   <si>
@@ -111,24 +99,6 @@
     <t>(1,2,3)</t>
   </si>
   <si>
-    <t>Buses</t>
-  </si>
-  <si>
-    <t>BusID(PK)</t>
-  </si>
-  <si>
-    <t>BusNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String </t>
-  </si>
-  <si>
-    <t>BusType</t>
-  </si>
-  <si>
-    <t>PlaceID(FK)</t>
-  </si>
-  <si>
     <t>Username(CK)</t>
   </si>
   <si>
@@ -141,15 +111,9 @@
     <t>PlaceId(FK)</t>
   </si>
   <si>
-    <t>Place_Bus_Mapping</t>
-  </si>
-  <si>
     <t>Place_Guide_Mapping</t>
   </si>
   <si>
-    <t>BusId(FK)</t>
-  </si>
-  <si>
     <t>UserId(PK, CK)</t>
   </si>
   <si>
@@ -280,6 +244,57 @@
   </si>
   <si>
     <t>DateTime</t>
+  </si>
+  <si>
+    <t>guide_type</t>
+  </si>
+  <si>
+    <t>number_of_people</t>
+  </si>
+  <si>
+    <t>pickup_date_time</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>Transporter_Master</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>contact_no</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>plate_no</t>
+  </si>
+  <si>
+    <t>city_id (FK)</t>
+  </si>
+  <si>
+    <t>pickup_location</t>
+  </si>
+  <si>
+    <t>Datetime</t>
+  </si>
+  <si>
+    <t>transporter_id(FK)</t>
+  </si>
+  <si>
+    <t>user_id(FK)</t>
+  </si>
+  <si>
+    <t>Transporte_Master</t>
   </si>
 </sst>
 </file>
@@ -331,7 +346,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -353,6 +368,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor rgb="FF666699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF284780"/>
         <bgColor rgb="FF666699"/>
       </patternFill>
     </fill>
@@ -412,20 +433,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -434,10 +449,19 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -515,6 +539,9 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FF284780"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -824,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:L54"/>
+  <dimension ref="B3:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28:L28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -843,22 +870,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="E3" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F3" s="6"/>
-      <c r="H3" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="6"/>
-      <c r="K3" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="L3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="E3" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="H3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="7"/>
+      <c r="K3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="7"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -874,13 +901,13 @@
         <v>2</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>2</v>
@@ -900,13 +927,13 @@
         <v>2</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>2</v>
@@ -929,18 +956,18 @@
       <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="H7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="5"/>
-      <c r="K7" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="L7" s="8"/>
+      <c r="E7" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="H7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="K7" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L7" s="6"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -950,19 +977,19 @@
         <v>2</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>2</v>
@@ -973,10 +1000,10 @@
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>2</v>
@@ -985,10 +1012,10 @@
         <v>37</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>2</v>
@@ -999,13 +1026,19 @@
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>2</v>
+        <v>82</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
@@ -1015,14 +1048,22 @@
       <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H11" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I11" s="8"/>
-      <c r="K11" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="L11" s="8"/>
+      <c r="E11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L11" s="6"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
@@ -1031,14 +1072,14 @@
       <c r="C12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>2</v>
+      <c r="E12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>2</v>
@@ -1046,105 +1087,105 @@
     </row>
     <row r="13" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="3"/>
-      <c r="H13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>84</v>
       </c>
+      <c r="F13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" s="4"/>
       <c r="K13" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="H14" s="2" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>84</v>
+        <v>2</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>31</v>
-      </c>
+    <row r="15" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E15" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" s="11"/>
       <c r="H15" s="2" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B16" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="6"/>
+      <c r="B16" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="7"/>
       <c r="E16" s="2" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="H16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="K16" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I17" s="8"/>
+        <v>86</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="K17" s="2" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>2</v>
@@ -1152,25 +1193,25 @@
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>2</v>
@@ -1178,19 +1219,19 @@
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I19" s="2" t="s">
+      <c r="E19" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>2</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>2</v>
@@ -1198,67 +1239,59 @@
     </row>
     <row r="20" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F20" s="6"/>
-      <c r="H20" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="E20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I20" s="6"/>
     </row>
     <row r="21" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="L21" s="8"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L21" s="6"/>
+    </row>
+    <row r="22" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="E22" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="6"/>
       <c r="H22" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>2</v>
@@ -1266,27 +1299,37 @@
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>57</v>
+        <v>45</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E24" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="8"/>
-      <c r="H24" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I24" s="8"/>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="K24" s="2" t="s">
         <v>4</v>
       </c>
@@ -1295,44 +1338,24 @@
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="K25" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B26" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="8"/>
-      <c r="E26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B26" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="E26" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="6"/>
       <c r="K26" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>2</v>
@@ -1340,17 +1363,15 @@
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E27"/>
-      <c r="F27"/>
-      <c r="H27" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I27" s="2" t="s">
+      <c r="E27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>2</v>
       </c>
       <c r="K27" s="1"/>
@@ -1358,31 +1379,33 @@
     </row>
     <row r="28" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E28"/>
-      <c r="F28"/>
-      <c r="K28" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="L28" s="10"/>
-    </row>
-    <row r="29" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="L28" s="9"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F29" s="8"/>
+      <c r="E29"/>
+      <c r="F29"/>
       <c r="K29" s="2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>2</v>
@@ -1390,59 +1413,137 @@
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="E30"/>
+      <c r="F30"/>
       <c r="K30" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" s="6"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="E37"/>
-      <c r="F37"/>
-    </row>
-    <row r="49" spans="5:6" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39"/>
+      <c r="F39"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40"/>
+      <c r="F40"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41"/>
+      <c r="F41"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42"/>
+      <c r="F42"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43"/>
+      <c r="F43"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44"/>
+      <c r="F44"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45"/>
+      <c r="F45"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46"/>
+      <c r="F46"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47"/>
+      <c r="F47"/>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48"/>
+      <c r="F48"/>
+    </row>
+    <row r="49" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E49"/>
       <c r="F49"/>
     </row>
@@ -1458,35 +1559,24 @@
       <c r="E52"/>
       <c r="F52"/>
     </row>
-    <row r="53" spans="5:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="E53"/>
-      <c r="F53"/>
-    </row>
-    <row r="54" spans="5:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="E54"/>
-      <c r="F54"/>
-    </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B16:C16"/>
+  <mergeCells count="16">
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="K3:L3"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E22:F22"/>
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="K28:L28"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="H20:I20"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="B16:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Database and entity modification
</commit_message>
<xml_diff>
--- a/DB_Structure.xlsx
+++ b/DB_Structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MscIT_SR\sem-projects\Sem8\Sprint1\TheLandmarkTour\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7381143-8314-495C-842B-8987EFB21E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D386F87B-775A-469E-BF38-66C39E5D7A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="99">
   <si>
     <t>Places</t>
   </si>
@@ -295,6 +295,33 @@
   </si>
   <si>
     <t>Transporte_Master</t>
+  </si>
+  <si>
+    <t>Event_Master</t>
+  </si>
+  <si>
+    <t>start_time</t>
+  </si>
+  <si>
+    <t>end_time</t>
+  </si>
+  <si>
+    <t>event_status</t>
+  </si>
+  <si>
+    <t>Event_user_Mapping</t>
+  </si>
+  <si>
+    <t>EventId(FK)</t>
+  </si>
+  <si>
+    <t>transport_id</t>
+  </si>
+  <si>
+    <t>transport_ID(FK)</t>
+  </si>
+  <si>
+    <t>integer</t>
   </si>
 </sst>
 </file>
@@ -433,16 +460,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -853,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23:L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -870,22 +891,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="E3" s="7" t="s">
+      <c r="C3" s="5"/>
+      <c r="E3" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="H3" s="7" t="s">
+      <c r="F3" s="5"/>
+      <c r="H3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="K3" s="7" t="s">
+      <c r="I3" s="5"/>
+      <c r="K3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="L3" s="7"/>
+      <c r="L3" s="5"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -956,18 +977,18 @@
       <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F7" s="11"/>
+      <c r="F7" s="9"/>
       <c r="H7" s="3" t="s">
         <v>34</v>
       </c>
       <c r="I7" s="4"/>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="L7" s="6"/>
+      <c r="L7" s="4"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -1060,10 +1081,10 @@
       <c r="I11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="K11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="L11" s="6"/>
+      <c r="L11" s="4"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
@@ -1124,10 +1145,10 @@
       </c>
     </row>
     <row r="15" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="F15" s="11"/>
+      <c r="F15" s="9"/>
       <c r="H15" s="2" t="s">
         <v>4</v>
       </c>
@@ -1142,10 +1163,10 @@
       </c>
     </row>
     <row r="16" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="7"/>
+      <c r="C16" s="5"/>
       <c r="E16" s="2" t="s">
         <v>79</v>
       </c>
@@ -1250,12 +1271,18 @@
       <c r="F20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I20" s="6"/>
-    </row>
-    <row r="21" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="I20" s="4"/>
+      <c r="K20" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>20</v>
       </c>
@@ -1268,10 +1295,12 @@
       <c r="I21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K21" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="L21" s="6"/>
+      <c r="K21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="22" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
@@ -1280,24 +1309,18 @@
       <c r="C22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="6"/>
+      <c r="F22" s="4"/>
       <c r="H22" s="2" t="s">
         <v>58</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>56</v>
       </c>
@@ -1316,12 +1339,10 @@
       <c r="I23" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K23" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="K23" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L23" s="4"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E24" s="2" t="s">
@@ -1331,7 +1352,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>2</v>
@@ -1339,23 +1360,27 @@
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="K25" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="E26" s="5" t="s">
+      <c r="C26" s="4"/>
+      <c r="E26" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="6"/>
+      <c r="F26" s="4"/>
+      <c r="H26" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I26" s="4"/>
       <c r="K26" s="2" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>2</v>
@@ -1374,10 +1399,20 @@
       <c r="F27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-    </row>
-    <row r="28" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H27" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>47</v>
       </c>
@@ -1390,10 +1425,18 @@
       <c r="F28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K28" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="L28" s="9"/>
+      <c r="H28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
@@ -1404,14 +1447,16 @@
       </c>
       <c r="E29"/>
       <c r="F29"/>
-      <c r="K29" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+    </row>
+    <row r="30" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
         <v>27</v>
       </c>
@@ -1420,12 +1465,16 @@
       </c>
       <c r="E30"/>
       <c r="F30"/>
-      <c r="K30" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="H30" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="L30" s="7"/>
     </row>
     <row r="31" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
@@ -1434,10 +1483,22 @@
       <c r="C31" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F31" s="6"/>
+      <c r="F31" s="4"/>
+      <c r="H31" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
@@ -1452,8 +1513,20 @@
       <c r="F32" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H32" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>65</v>
       </c>
@@ -1466,8 +1539,14 @@
       <c r="F33" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H33" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>73</v>
       </c>
@@ -1475,75 +1554,101 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B35" s="2" t="s">
         <v>74</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H35" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H37" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39"/>
       <c r="F39"/>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40"/>
       <c r="F40"/>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41"/>
       <c r="F41"/>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42"/>
       <c r="F42"/>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43"/>
       <c r="F43"/>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44"/>
       <c r="F44"/>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45"/>
       <c r="F45"/>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46"/>
       <c r="F46"/>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47"/>
       <c r="F47"/>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48"/>
       <c r="F48"/>
     </row>
-    <row r="49" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:6" ht="15" x14ac:dyDescent="0.25">
       <c r="E49"/>
       <c r="F49"/>
     </row>
@@ -1560,14 +1665,18 @@
       <c r="F52"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="20">
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="K23:L23"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="E22:F22"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="K30:L30"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="B3:C3"/>

</xml_diff>

<commit_message>
Bugfix: Switch profile, My trip rendering/ data fetching issue due to scope (beta), validation fixes, other modifications
</commit_message>
<xml_diff>
--- a/DB_Structure.xlsx
+++ b/DB_Structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MscIT_SR\sem-projects\Sem8\Sprint1\TheLandmarkTour\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D386F87B-775A-469E-BF38-66C39E5D7A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F6D18E-08DF-4E17-A9D6-7990087253CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1666,11 +1666,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="K23:L23"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="E31:F31"/>
@@ -1686,6 +1681,11 @@
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="B16:C16"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="K23:L23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>